<commit_message>
cambios en los datos y limpieza a las columnas edad, estado, numero
</commit_message>
<xml_diff>
--- a/data/Información de contacto (Respuestas).xlsx
+++ b/data/Información de contacto (Respuestas).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="101">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -296,6 +296,24 @@
   </si>
   <si>
     <t>Game of Thrones, Friends, Heartstopper</t>
+  </si>
+  <si>
+    <t>valc941226@gmail.com</t>
+  </si>
+  <si>
+    <t>José Carlos</t>
+  </si>
+  <si>
+    <t>Ocho</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Clásica, Rock, Jazz</t>
+  </si>
+  <si>
+    <t>BCS, One Piece, Malcom</t>
   </si>
 </sst>
 </file>
@@ -1218,6 +1236,44 @@
         <v>32</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" s="2">
+        <v>44840.866328449076</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K17" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0.9791666666642413</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>